<commit_message>
Updated regression slides and examples
</commit_message>
<xml_diff>
--- a/slides/regression.xlsx
+++ b/slides/regression.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_cmps460-content\slides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFDABA0-0766-4BDD-9B5C-7312D35C4F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303AFF2A-7056-472B-8983-CE9E2094E9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4DB60BD1-2AA0-4BE9-AF0B-E8DCF890EA2E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{4DB60BD1-2AA0-4BE9-AF0B-E8DCF890EA2E}"/>
   </bookViews>
   <sheets>
-    <sheet name="lr" sheetId="2" r:id="rId1"/>
+    <sheet name="regression" sheetId="2" r:id="rId1"/>
+    <sheet name="x^2" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="Actual">'[1]Auto Correlation'!$C$4:$C$123</definedName>
@@ -59,9 +60,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
-    <t>Y-Intercept:</t>
-  </si>
-  <si>
     <t>Avg Daily Temp:</t>
   </si>
   <si>
@@ -80,46 +78,16 @@
     <t>Error ^2</t>
   </si>
   <si>
-    <t>Show Line</t>
-  </si>
-  <si>
-    <t>Avg Temp (˚C)</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Prediction</t>
-  </si>
-  <si>
-    <t>Line Slope:</t>
-  </si>
-  <si>
     <t>Forecasted Sales:</t>
   </si>
   <si>
-    <t>Show OLS</t>
-  </si>
-  <si>
-    <t>Show Trend</t>
-  </si>
-  <si>
-    <t>Show Forecast</t>
-  </si>
-  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Slope Value:</t>
   </si>
   <si>
     <t>Ice cream sales</t>
   </si>
   <si>
     <t>Best</t>
-  </si>
-  <si>
-    <t>Slope: 0.6958 &amp; Intercept: 10.867</t>
   </si>
   <si>
     <t>MSE</t>
@@ -129,21 +97,53 @@
 </t>
   </si>
   <si>
-    <t>Y-Intercept (w)</t>
+    <t>Prediction y_hat</t>
   </si>
   <si>
-    <t>Data for Chart</t>
+    <t>Y-Intercept (b):</t>
+  </si>
+  <si>
+    <t>Line Slope (w):</t>
+  </si>
+  <si>
+    <t>Slope (w)</t>
+  </si>
+  <si>
+    <t>Avg Temp (˚C) -  x</t>
+  </si>
+  <si>
+    <t>Sales - y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x ^ 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m = </t>
+  </si>
+  <si>
+    <t>Suppose we lock b = 10.87</t>
+  </si>
+  <si>
+    <t>Data for plots</t>
+  </si>
+  <si>
+    <t>Diff Data</t>
+  </si>
+  <si>
+    <t>Slope: 0.7 &amp; Intercept: 10.87</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,8 +275,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="0.39997558519241921"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,6 +348,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,7 +495,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -508,7 +522,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,9 +537,6 @@
     <xf numFmtId="4" fontId="2" fillId="5" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="8" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -541,6 +551,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="7" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -565,19 +593,16 @@
     <xf numFmtId="1" fontId="12" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,10 +672,12 @@
             <c:size val="7"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="37E5F7"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="12700">
-                <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -711,7 +738,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>lr!$Y$3:$Y$13</c:f>
+              <c:f>regression!$Z$4:$Z$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -753,10 +780,13 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>lr!$AA$3:$AA$13</c:f>
+              <c:f>regression!$AB$4:$AB$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
                 </c:pt>
@@ -806,7 +836,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FFFF89"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -823,7 +853,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>lr!$Y$3:$Y$13</c:f>
+              <c:f>regression!$Z$4:$Z$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -865,42 +895,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>lr!$Z$3:$Z$13</c:f>
+              <c:f>regression!$AA$4:$AA$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.5</c:v>
+                  <c:v>14.37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>17.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.5</c:v>
+                  <c:v>21.369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21</c:v>
+                  <c:v>24.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.5</c:v>
+                  <c:v>28.369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>31.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.5</c:v>
+                  <c:v>35.369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35</c:v>
+                  <c:v>38.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>38.5</c:v>
+                  <c:v>42.37</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42</c:v>
+                  <c:v>45.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -919,11 +949,10 @@
             <c:v>Diff</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="37E5F7"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1133,7 +1162,7 @@
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>lr!$Y$17:$Y$38</c:f>
+              <c:f>regression!$X$3:$X$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -1208,72 +1237,72 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>lr!$Z$17:$Z$38</c:f>
+              <c:f>regression!$Y$3:$Y$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>7</c:v>
+                <c:pt idx="0" formatCode="#,##0.00">
+                  <c:v>10.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.5</c:v>
+                <c:pt idx="2" formatCode="#,##0.00">
+                  <c:v>14.37</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>14</c:v>
+                <c:pt idx="4" formatCode="#,##0.00">
+                  <c:v>17.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>17.5</c:v>
+                <c:pt idx="6" formatCode="#,##0.00">
+                  <c:v>21.369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>21</c:v>
+                <c:pt idx="8" formatCode="#,##0.00">
+                  <c:v>24.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>24.5</c:v>
+                <c:pt idx="10" formatCode="#,##0.00">
+                  <c:v>28.369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>28</c:v>
+                <c:pt idx="12" formatCode="#,##0.00">
+                  <c:v>31.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>31.5</c:v>
+                <c:pt idx="14" formatCode="#,##0.00">
+                  <c:v>35.369999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>35</c:v>
+                <c:pt idx="16" formatCode="#,##0.00">
+                  <c:v>38.869999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>38.5</c:v>
+                <c:pt idx="18" formatCode="#,##0.00">
+                  <c:v>42.37</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>42</c:v>
+                <c:pt idx="20" formatCode="#,##0.00">
+                  <c:v>45.87</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>34</c:v>
@@ -1560,9 +1589,8 @@
       </c:valAx>
       <c:spPr>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:ln>
@@ -1665,7 +1693,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>lr!$C$22</c:f>
+              <c:f>regression!$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1698,7 +1726,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>lr!$B$23:$B$41</c:f>
+              <c:f>regression!$B$24:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1764,66 +1792,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>lr!$C$23:$C$41</c:f>
+              <c:f>regression!$C$24:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>808.5</c:v>
+                  <c:v>731.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>645.4</c:v>
+                  <c:v>583.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>501.4</c:v>
+                  <c:v>453.42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>376.8</c:v>
+                  <c:v>340.42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>271.3</c:v>
+                  <c:v>244.93</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>185.2</c:v>
+                  <c:v>166.94</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>118.2</c:v>
+                  <c:v>106.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.599999999999994</c:v>
+                  <c:v>63.46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.2</c:v>
+                  <c:v>37.97</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33</c:v>
+                  <c:v>29.98</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43</c:v>
+                  <c:v>39.49</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>72.400000000000006</c:v>
+                  <c:v>66.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120.9</c:v>
+                  <c:v>111.01</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>188.8</c:v>
+                  <c:v>173.02</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>275.8</c:v>
+                  <c:v>252.52</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>382.2</c:v>
+                  <c:v>349.53</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>507.7</c:v>
+                  <c:v>464.04</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>652.6</c:v>
+                  <c:v>496.05</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>816.6</c:v>
+                  <c:v>745.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2133,7 +2161,468 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'x^2'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>x ^ 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'x^2'!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'x^2'!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A6E-4BF0-A854-FE55327D1BF9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1481579743"/>
+        <c:axId val="1431759472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1481579743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1431759472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1431759472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1481579743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2173,7 +2662,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3245,8 +3734,524 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$2" max="50" page="10" val="7"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="26" fmlaLink="$I$2" max="50" page="10" val="10"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3277,8 +4282,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4586967" y="942793"/>
-          <a:ext cx="10152743" cy="4164421"/>
+          <a:off x="5332185" y="1074329"/>
+          <a:ext cx="10143672" cy="4069171"/>
           <a:chOff x="402697" y="943848"/>
           <a:chExt cx="10451840" cy="4395954"/>
         </a:xfrm>
@@ -3325,35 +4330,20 @@
           <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
+          <a:ln/>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+            <a:schemeClr val="accent2"/>
           </a:lnRef>
           <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="lt1"/>
           </a:fillRef>
           <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
+            <a:schemeClr val="accent2"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="dk1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
@@ -3373,7 +4363,7 @@
                 <a:cs typeface="Calibri"/>
               </a:rPr>
               <a:pPr algn="ctr"/>
-              <a:t>y = 0.7x + 7</a:t>
+              <a:t>y = 0.7x + 10.87</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="6600" b="1" i="0">
               <a:solidFill>
@@ -3400,7 +4390,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>9</xdr:col>
-          <xdr:colOff>304800</xdr:colOff>
+          <xdr:colOff>311150</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3470,6 +4460,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>231775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -30698,17 +31729,17 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:AB41"/>
+  <dimension ref="B1:AB42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:C22"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.31640625" customWidth="1"/>
+    <col min="2" max="2" width="19.953125" customWidth="1"/>
+    <col min="4" max="4" width="15.86328125" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="10.31640625" customWidth="1"/>
     <col min="7" max="7" width="11.453125" customWidth="1"/>
@@ -30718,845 +31749,853 @@
     <col min="14" max="14" width="10.453125" customWidth="1"/>
     <col min="15" max="15" width="6.453125" customWidth="1"/>
     <col min="16" max="16" width="5.54296875" customWidth="1"/>
-    <col min="25" max="26" width="8.54296875" customWidth="1"/>
-    <col min="27" max="27" width="9.54296875" customWidth="1"/>
-    <col min="28" max="28" width="8.54296875" customWidth="1"/>
+    <col min="23" max="25" width="0" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="8.54296875" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="9.54296875" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="21" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="Y1" s="23" t="s">
-        <v>24</v>
+      <c r="X1" s="38" t="s">
+        <v>23</v>
       </c>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
     </row>
     <row r="2" spans="2:28" ht="20.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="24" t="s">
-        <v>18</v>
+      <c r="B2" s="30" t="s">
+        <v>8</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="27">
+        <f>COUNT(B4:B14)</f>
+        <v>11</v>
+      </c>
       <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2">
+        <v>10.87</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="39">
+        <f>F15</f>
+        <v>29.978999999999999</v>
+      </c>
+      <c r="L2" s="40"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2">
+      <c r="O2" s="33">
+        <v>13</v>
+      </c>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="4"/>
+      <c r="X2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="31">
-        <f>F14</f>
-        <v>47.024999999999999</v>
-      </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="1" t="s">
+      <c r="Z2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="27">
-        <v>40</v>
-      </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="4"/>
-      <c r="Y2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AB2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="6" t="s">
+    </row>
+    <row r="3" spans="2:28" ht="30.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:28" ht="20.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.75">
-      <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>6</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I3" s="8">
         <v>0.7</v>
       </c>
-      <c r="J3" s="26"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="40"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="35">
         <f>IF(ISBLANK(O2),"",(O2*I3)+I2)</f>
-        <v>35</v>
+        <v>19.97</v>
       </c>
-      <c r="P3" s="30"/>
+      <c r="P3" s="36"/>
       <c r="Q3" s="4"/>
-      <c r="Y3" s="5">
+      <c r="X3" s="5">
+        <f>B4</f>
         <v>0</v>
       </c>
-      <c r="Z3" s="5">
-        <f>IF($AB$3=TRUE,I2,NA())</f>
-        <v>7</v>
-      </c>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="10" t="b">
-        <v>1</v>
+      <c r="Y3" s="37">
+        <f>$D$4</f>
+        <v>10.87</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B4" s="11">
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
         <v>5</v>
       </c>
-      <c r="C4" s="11">
-        <v>8</v>
+      <c r="D4" s="28">
+        <f>($I$3*B4) + $I$2</f>
+        <v>10.87</v>
       </c>
-      <c r="D4" s="16">
-        <f>($I$3*B4) + $I$2</f>
-        <v>10.5</v>
+      <c r="E4" s="16">
+        <f>D4 - C4</f>
+        <v>5.8699999999999992</v>
       </c>
-      <c r="E4" s="18">
-        <f>D4 - C4</f>
-        <v>2.5</v>
+      <c r="F4" s="18">
+        <f>E4 ^2</f>
+        <v>34.45689999999999</v>
       </c>
-      <c r="F4" s="20">
-        <f>E4 ^2</f>
-        <v>6.25</v>
+      <c r="I4" s="11" t="str">
+        <f>"y = "&amp;I3&amp;"x + "&amp;I2</f>
+        <v>y = 0.7x + 10.87</v>
       </c>
-      <c r="I4" s="12" t="str">
-        <f>"y = "&amp;I3&amp;"x + "&amp;I2</f>
-        <v>y = 0.7x + 7</v>
+      <c r="J4" s="12"/>
+      <c r="X4" s="5">
+        <f>B4</f>
+        <v>0</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="Y4" s="5">
+      <c r="Y4" s="13">
+        <f>$C$4</f>
         <v>5</v>
       </c>
       <c r="Z4" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y4)+$I$2,NA())</f>
-        <v>10.5</v>
+        <f>B4</f>
+        <v>0</v>
       </c>
       <c r="AA4" s="5">
+        <f>($I$3*$Z4)+$I$2</f>
+        <v>10.87</v>
+      </c>
+      <c r="AB4" s="9">
+        <f>C4</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:28" ht="14.9" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="B5" s="10">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10">
         <v>8</v>
       </c>
-      <c r="AB4" s="10"/>
-    </row>
-    <row r="5" spans="2:28" ht="14.9" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="11">
-        <v>10</v>
+      <c r="D5" s="28">
+        <f>($I$3*B5) + $I$2</f>
+        <v>14.37</v>
       </c>
-      <c r="C5" s="11">
-        <v>16</v>
+      <c r="E5" s="16">
+        <f>D5 - C5</f>
+        <v>6.3699999999999992</v>
       </c>
-      <c r="D5" s="16">
-        <f t="shared" ref="D5:D13" si="0">($I$3*B5) + $I$2</f>
-        <v>14</v>
+      <c r="F5" s="18">
+        <f>E5 ^2</f>
+        <v>40.576899999999988</v>
       </c>
-      <c r="E5" s="18">
-        <f t="shared" ref="E5:E13" si="1">D5 - C5</f>
-        <v>-2</v>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="X5" s="5">
+        <f>B5</f>
+        <v>5</v>
       </c>
-      <c r="F5" s="20">
-        <f t="shared" ref="F5:F13" si="2">E5 ^2</f>
-        <v>4</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="Y5" s="5">
-        <v>10</v>
+      <c r="Y5" s="37">
+        <f>$D$5</f>
+        <v>14.37</v>
       </c>
       <c r="Z5" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y5)+$I$2,NA())</f>
-        <v>14</v>
+        <f t="shared" ref="Z5:Z14" si="0">B5</f>
+        <v>5</v>
       </c>
       <c r="AA5" s="5">
-        <v>16</v>
+        <f>($I$3*$Z5)+$I$2</f>
+        <v>14.37</v>
       </c>
-      <c r="AB5" s="10" t="s">
-        <v>13</v>
+      <c r="AB5" s="9">
+        <f t="shared" ref="AB5:AB14" si="1">C5</f>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B6" s="11">
-        <v>15</v>
+      <c r="B6" s="10">
+        <v>10</v>
       </c>
-      <c r="C6" s="11">
-        <v>19</v>
+      <c r="C6" s="10">
+        <v>16</v>
       </c>
-      <c r="D6" s="16">
-        <f t="shared" si="0"/>
-        <v>17.5</v>
+      <c r="D6" s="28">
+        <f t="shared" ref="D6:D14" si="2">($I$3*B6) + $I$2</f>
+        <v>17.869999999999997</v>
       </c>
-      <c r="E6" s="18">
-        <f t="shared" si="1"/>
-        <v>-1.5</v>
+      <c r="E6" s="16">
+        <f t="shared" ref="E6:E14" si="3">D6 - C6</f>
+        <v>1.8699999999999974</v>
       </c>
-      <c r="F6" s="20">
-        <f t="shared" si="2"/>
-        <v>2.25</v>
+      <c r="F6" s="18">
+        <f t="shared" ref="F6:F14" si="4">E6 ^2</f>
+        <v>3.4968999999999903</v>
       </c>
-      <c r="Y6" s="5">
-        <v>15</v>
+      <c r="X6" s="5">
+        <f>B5</f>
+        <v>5</v>
+      </c>
+      <c r="Y6" s="13">
+        <f>$C$5</f>
+        <v>8</v>
       </c>
       <c r="Z6" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y6)+$I$2,NA())</f>
-        <v>17.5</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="AA6" s="5">
-        <v>19</v>
+        <f>($I$3*$Z6)+$I$2</f>
+        <v>17.869999999999997</v>
       </c>
-      <c r="AB6" s="10" t="b">
-        <v>1</v>
+      <c r="AB6" s="9">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B7" s="11">
+      <c r="B7" s="10">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10">
+        <v>19</v>
+      </c>
+      <c r="D7" s="28">
+        <f t="shared" si="2"/>
+        <v>21.369999999999997</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" si="3"/>
+        <v>2.3699999999999974</v>
+      </c>
+      <c r="F7" s="18">
+        <f t="shared" si="4"/>
+        <v>5.6168999999999878</v>
+      </c>
+      <c r="X7" s="5">
+        <f>B6</f>
+        <v>10</v>
+      </c>
+      <c r="Y7" s="37">
+        <f>$D$6</f>
+        <v>17.869999999999997</v>
+      </c>
+      <c r="Z7" s="5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="AA7" s="5">
+        <f>($I$3*$Z7)+$I$2</f>
+        <v>21.369999999999997</v>
+      </c>
+      <c r="AB7" s="9">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.75">
+      <c r="B8" s="10">
         <v>20</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C8" s="10">
         <v>30</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D8" s="28">
+        <f t="shared" si="2"/>
+        <v>24.869999999999997</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="3"/>
+        <v>-5.1300000000000026</v>
+      </c>
+      <c r="F8" s="18">
+        <f t="shared" si="4"/>
+        <v>26.316900000000025</v>
+      </c>
+      <c r="X8" s="5">
+        <f>B6</f>
+        <v>10</v>
+      </c>
+      <c r="Y8" s="13">
+        <f>$C$6</f>
+        <v>16</v>
+      </c>
+      <c r="Z8" s="5">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="E7" s="18">
-        <f t="shared" si="1"/>
-        <v>-9</v>
-      </c>
-      <c r="F7" s="20">
-        <f t="shared" si="2"/>
-        <v>81</v>
-      </c>
-      <c r="Y7" s="5">
         <v>20</v>
       </c>
-      <c r="Z7" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y7)+$I$2,NA())</f>
-        <v>21</v>
+      <c r="AA8" s="5">
+        <f>($I$3*$Z8)+$I$2</f>
+        <v>24.869999999999997</v>
       </c>
-      <c r="AA7" s="5">
+      <c r="AB8" s="9">
+        <f t="shared" si="1"/>
         <v>30</v>
-      </c>
-      <c r="AB7" s="10"/>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B8" s="11">
-        <v>25</v>
-      </c>
-      <c r="C8" s="11">
-        <v>35</v>
-      </c>
-      <c r="D8" s="16">
-        <f t="shared" si="0"/>
-        <v>24.5</v>
-      </c>
-      <c r="E8" s="18">
-        <f t="shared" si="1"/>
-        <v>-10.5</v>
-      </c>
-      <c r="F8" s="20">
-        <f t="shared" si="2"/>
-        <v>110.25</v>
-      </c>
-      <c r="Y8" s="5">
-        <v>25</v>
-      </c>
-      <c r="Z8" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y8)+$I$2,NA())</f>
-        <v>24.5</v>
-      </c>
-      <c r="AA8" s="5">
-        <v>35</v>
-      </c>
-      <c r="AB8" s="10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B9" s="11">
-        <v>30</v>
+      <c r="B9" s="10">
+        <v>25</v>
       </c>
-      <c r="C9" s="11">
-        <v>30</v>
+      <c r="C9" s="10">
+        <v>35</v>
       </c>
-      <c r="D9" s="16">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="D9" s="28">
+        <f t="shared" si="2"/>
+        <v>28.369999999999997</v>
       </c>
-      <c r="E9" s="18">
-        <f t="shared" si="1"/>
-        <v>-2</v>
+      <c r="E9" s="16">
+        <f t="shared" si="3"/>
+        <v>-6.6300000000000026</v>
       </c>
-      <c r="F9" s="20">
-        <f t="shared" si="2"/>
-        <v>4</v>
+      <c r="F9" s="18">
+        <f t="shared" si="4"/>
+        <v>43.956900000000033</v>
       </c>
-      <c r="Y9" s="5">
-        <v>30</v>
+      <c r="X9" s="5">
+        <f>B7</f>
+        <v>15</v>
+      </c>
+      <c r="Y9" s="37">
+        <f>$D$7</f>
+        <v>21.369999999999997</v>
       </c>
       <c r="Z9" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y9)+$I$2,NA())</f>
-        <v>28</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="AA9" s="5">
-        <v>30</v>
+        <f>($I$3*$Z9)+$I$2</f>
+        <v>28.369999999999997</v>
       </c>
-      <c r="AB9" s="10" t="b">
-        <v>0</v>
+      <c r="AB9" s="9">
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B10" s="11">
+      <c r="B10" s="10">
+        <v>30</v>
+      </c>
+      <c r="C10" s="10">
+        <v>30</v>
+      </c>
+      <c r="D10" s="28">
+        <f t="shared" si="2"/>
+        <v>31.869999999999997</v>
+      </c>
+      <c r="E10" s="16">
+        <f t="shared" si="3"/>
+        <v>1.8699999999999974</v>
+      </c>
+      <c r="F10" s="18">
+        <f t="shared" si="4"/>
+        <v>3.4968999999999903</v>
+      </c>
+      <c r="X10" s="5">
+        <f>B7</f>
+        <v>15</v>
+      </c>
+      <c r="Y10" s="13">
+        <f>$C$7</f>
+        <v>19</v>
+      </c>
+      <c r="Z10" s="5">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AA10" s="5">
+        <f>($I$3*$Z10)+$I$2</f>
+        <v>31.869999999999997</v>
+      </c>
+      <c r="AB10" s="9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.75">
+      <c r="B11" s="10">
         <v>35</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C11" s="10">
         <v>43</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D11" s="28">
+        <f t="shared" si="2"/>
+        <v>35.369999999999997</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="3"/>
+        <v>-7.6300000000000026</v>
+      </c>
+      <c r="F11" s="18">
+        <f t="shared" si="4"/>
+        <v>58.216900000000038</v>
+      </c>
+      <c r="X11" s="5">
+        <f>B8</f>
+        <v>20</v>
+      </c>
+      <c r="Y11" s="37">
+        <f>$D$8</f>
+        <v>24.869999999999997</v>
+      </c>
+      <c r="Z11" s="5">
         <f t="shared" si="0"/>
-        <v>31.5</v>
-      </c>
-      <c r="E10" s="18">
-        <f t="shared" si="1"/>
-        <v>-11.5</v>
-      </c>
-      <c r="F10" s="20">
-        <f t="shared" si="2"/>
-        <v>132.25</v>
-      </c>
-      <c r="Y10" s="5">
         <v>35</v>
       </c>
-      <c r="Z10" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y10)+$I$2,NA())</f>
-        <v>31.5</v>
+      <c r="AA11" s="5">
+        <f>($I$3*$Z11)+$I$2</f>
+        <v>35.369999999999997</v>
       </c>
-      <c r="AA10" s="5">
+      <c r="AB11" s="9">
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B11" s="11">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.75">
+      <c r="B12" s="10">
         <v>40</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C12" s="10">
         <v>41</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D12" s="28">
+        <f t="shared" si="2"/>
+        <v>38.869999999999997</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="3"/>
+        <v>-2.1300000000000026</v>
+      </c>
+      <c r="F12" s="18">
+        <f t="shared" si="4"/>
+        <v>4.5369000000000108</v>
+      </c>
+      <c r="X12" s="5">
+        <f>B8</f>
+        <v>20</v>
+      </c>
+      <c r="Y12" s="13">
+        <f>$C$8</f>
+        <v>30</v>
+      </c>
+      <c r="Z12" s="5">
         <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="E11" s="18">
-        <f t="shared" si="1"/>
-        <v>-6</v>
-      </c>
-      <c r="F11" s="20">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="Y11" s="5">
         <v>40</v>
       </c>
-      <c r="Z11" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y11)+$I$2,NA())</f>
-        <v>35</v>
+      <c r="AA12" s="5">
+        <f>($I$3*$Z12)+$I$2</f>
+        <v>38.869999999999997</v>
       </c>
-      <c r="AA11" s="5">
+      <c r="AB12" s="9">
+        <f t="shared" si="1"/>
         <v>41</v>
-      </c>
-      <c r="AB11" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B12" s="11">
-        <v>45</v>
-      </c>
-      <c r="C12" s="11">
-        <v>44</v>
-      </c>
-      <c r="D12" s="16">
-        <f t="shared" si="0"/>
-        <v>38.5</v>
-      </c>
-      <c r="E12" s="18">
-        <f t="shared" si="1"/>
-        <v>-5.5</v>
-      </c>
-      <c r="F12" s="20">
-        <f t="shared" si="2"/>
-        <v>30.25</v>
-      </c>
-      <c r="Y12" s="5">
-        <v>45</v>
-      </c>
-      <c r="Z12" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y12)+$I$2,NA())</f>
-        <v>38.5</v>
-      </c>
-      <c r="AA12" s="5">
-        <v>44</v>
-      </c>
-      <c r="AB12" s="10" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B13" s="11">
+      <c r="B13" s="10">
+        <v>45</v>
+      </c>
+      <c r="C13" s="10">
+        <v>44</v>
+      </c>
+      <c r="D13" s="28">
+        <f t="shared" si="2"/>
+        <v>42.37</v>
+      </c>
+      <c r="E13" s="16">
+        <f t="shared" si="3"/>
+        <v>-1.6300000000000026</v>
+      </c>
+      <c r="F13" s="18">
+        <f t="shared" si="4"/>
+        <v>2.6569000000000083</v>
+      </c>
+      <c r="X13" s="5">
+        <f>B9</f>
+        <v>25</v>
+      </c>
+      <c r="Y13" s="37">
+        <f>$D$9</f>
+        <v>28.369999999999997</v>
+      </c>
+      <c r="Z13" s="5">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AA13" s="5">
+        <f>($I$3*$Z13)+$I$2</f>
+        <v>42.37</v>
+      </c>
+      <c r="AB13" s="9">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.75">
+      <c r="B14" s="10">
         <v>50</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C14" s="10">
         <v>34</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D14" s="28">
+        <f t="shared" si="2"/>
+        <v>45.87</v>
+      </c>
+      <c r="E14" s="16">
+        <f t="shared" si="3"/>
+        <v>11.869999999999997</v>
+      </c>
+      <c r="F14" s="18">
+        <f t="shared" si="4"/>
+        <v>140.89689999999993</v>
+      </c>
+      <c r="X14" s="5">
+        <f>B9</f>
+        <v>25</v>
+      </c>
+      <c r="Y14" s="13">
+        <f>$C$9</f>
+        <v>35</v>
+      </c>
+      <c r="Z14" s="5">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="E13" s="18">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="F13" s="20">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
-      <c r="Y13" s="5">
         <v>50</v>
       </c>
-      <c r="Z13" s="5">
-        <f>IF($AB$3=TRUE,($I$3*$Y13)+$I$2,NA())</f>
-        <v>42</v>
+      <c r="AA14" s="5">
+        <f>($I$3*$Z14)+$I$2</f>
+        <v>45.87</v>
       </c>
-      <c r="AA13" s="5">
+      <c r="AB14" s="9">
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="E14" s="21" t="s">
+    <row r="15" spans="2:28" x14ac:dyDescent="0.75">
+      <c r="E15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="20">
+        <f>SUM(F5:F14)/11</f>
+        <v>29.978999999999999</v>
+      </c>
+      <c r="X15" s="5">
+        <f>B10</f>
+        <v>30</v>
+      </c>
+      <c r="Y15" s="37">
+        <f>$D$10</f>
+        <v>31.869999999999997</v>
+      </c>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="5"/>
+      <c r="AB15" s="13"/>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.75">
+      <c r="X16" s="5">
+        <f>B10</f>
+        <v>30</v>
+      </c>
+      <c r="Y16" s="13">
+        <f>$C$10</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B17" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="X17" s="5">
+        <f>B11</f>
+        <v>35</v>
+      </c>
+      <c r="Y17" s="37">
+        <f>$D$11</f>
+        <v>35.369999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B18" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="X18" s="5">
+        <f>B11</f>
+        <v>35</v>
+      </c>
+      <c r="Y18" s="13">
+        <f>$C$11</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="X19" s="5">
+        <f>B12</f>
+        <v>40</v>
+      </c>
+      <c r="Y19" s="37">
+        <f>$D$12</f>
+        <v>38.869999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="X20" s="5">
+        <f>B12</f>
+        <v>40</v>
+      </c>
+      <c r="Y20" s="13">
+        <f>$C$12</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="X21" s="5">
+        <f>B13</f>
+        <v>45</v>
+      </c>
+      <c r="Y21" s="37">
+        <f>$D$13</f>
+        <v>42.37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B22" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="22">
-        <f>SUM(F4:F13)/10</f>
-        <v>47.024999999999999</v>
+      <c r="X22" s="5">
+        <f>B13</f>
+        <v>45</v>
       </c>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="14"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="Y15" s="5"/>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="14"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.75">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA16" s="10" t="s">
-        <v>17</v>
+      <c r="Y22" s="13">
+        <f>$C$13</f>
+        <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B17" s="33" t="s">
-        <v>20</v>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B23" s="24" t="s">
+        <v>15</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="Y17" s="5">
+      <c r="C23" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="X23" s="5">
+        <f>B14</f>
+        <v>50</v>
+      </c>
+      <c r="Y23" s="37">
+        <f>$D$14</f>
+        <v>45.87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B24" s="22">
+        <v>-0.2</v>
+      </c>
+      <c r="C24" s="22">
+        <v>731.9</v>
+      </c>
+      <c r="X24" s="5">
+        <f>B14</f>
+        <v>50</v>
+      </c>
+      <c r="Y24" s="13">
+        <f>$C$14</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B25" s="22">
+        <v>-0.1</v>
+      </c>
+      <c r="C25" s="22">
+        <v>583.91</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B26" s="22">
         <v>0</v>
       </c>
-      <c r="Z17" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y17,$Y$3:$AA$13,COUNTIF($Y$17:Y17,Y17)+1,0)=0,NA(),VLOOKUP($Y17,$Y$3:$AA$13,COUNTIF($Y$17:Y17,Y17)+1,0)),NA())</f>
-        <v>7</v>
-      </c>
-      <c r="AA17" s="6">
-        <v>54</v>
+      <c r="C26" s="22">
+        <v>453.42</v>
       </c>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="Y18" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="5" t="e">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y18,$Y$3:$AA$13,COUNTIF($Y$17:Y18,Y18)+1,0)=0,NA(),VLOOKUP($Y18,$Y$3:$AA$13,COUNTIF($Y$17:Y18,Y18)+1,0)),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AA18" s="14"/>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="Y19" s="5">
-        <v>5</v>
-      </c>
-      <c r="Z19" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y19,$Y$3:$AA$13,COUNTIF($Y$17:Y19,Y19)+1,0)=0,NA(),VLOOKUP($Y19,$Y$3:$AA$13,COUNTIF($Y$17:Y19,Y19)+1,0)),NA())</f>
-        <v>10.5</v>
-      </c>
-      <c r="AA19" s="14"/>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="Y20" s="5">
-        <v>5</v>
-      </c>
-      <c r="Z20" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y20,$Y$3:$AA$13,COUNTIF($Y$17:Y20,Y20)+1,0)=0,NA(),VLOOKUP($Y20,$Y$3:$AA$13,COUNTIF($Y$17:Y20,Y20)+1,0)),NA())</f>
-        <v>8</v>
-      </c>
-      <c r="AA20" s="14"/>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="Y21" s="5">
-        <v>10</v>
-      </c>
-      <c r="Z21" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y21,$Y$3:$AA$13,COUNTIF($Y$17:Y21,Y21)+1,0)=0,NA(),VLOOKUP($Y21,$Y$3:$AA$13,COUNTIF($Y$17:Y21,Y21)+1,0)),NA())</f>
-        <v>14</v>
-      </c>
-      <c r="AA21" s="14"/>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B22" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y22" s="5">
-        <v>10</v>
-      </c>
-      <c r="Z22" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y22,$Y$3:$AA$13,COUNTIF($Y$17:Y22,Y22)+1,0)=0,NA(),VLOOKUP($Y22,$Y$3:$AA$13,COUNTIF($Y$17:Y22,Y22)+1,0)),NA())</f>
-        <v>16</v>
-      </c>
-      <c r="AA22" s="14"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B23" s="34">
-        <v>-0.2</v>
-      </c>
-      <c r="C23" s="34">
-        <f>8085/10</f>
-        <v>808.5</v>
-      </c>
-      <c r="Y23" s="5">
-        <v>15</v>
-      </c>
-      <c r="Z23" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y23,$Y$3:$AA$13,COUNTIF($Y$17:Y23,Y23)+1,0)=0,NA(),VLOOKUP($Y23,$Y$3:$AA$13,COUNTIF($Y$17:Y23,Y23)+1,0)),NA())</f>
-        <v>17.5</v>
-      </c>
-      <c r="AA23" s="14"/>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B24" s="34">
-        <v>-0.1</v>
-      </c>
-      <c r="C24" s="34">
-        <f>6454/10</f>
-        <v>645.4</v>
-      </c>
-      <c r="Y24" s="5">
-        <v>15</v>
-      </c>
-      <c r="Z24" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y24,$Y$3:$AA$13,COUNTIF($Y$17:Y24,Y24)+1,0)=0,NA(),VLOOKUP($Y24,$Y$3:$AA$13,COUNTIF($Y$17:Y24,Y24)+1,0)),NA())</f>
-        <v>19</v>
-      </c>
-      <c r="AA24" s="14"/>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B25" s="34">
-        <v>0</v>
-      </c>
-      <c r="C25" s="34">
-        <f>5014/10</f>
-        <v>501.4</v>
-      </c>
-      <c r="Y25" s="5">
-        <v>20</v>
-      </c>
-      <c r="Z25" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y25,$Y$3:$AA$13,COUNTIF($Y$17:Y25,Y25)+1,0)=0,NA(),VLOOKUP($Y25,$Y$3:$AA$13,COUNTIF($Y$17:Y25,Y25)+1,0)),NA())</f>
-        <v>21</v>
-      </c>
-      <c r="AA25" s="14"/>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B26" s="34">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B27" s="22">
         <v>0.1</v>
       </c>
-      <c r="C26" s="34">
-        <f>3768/10</f>
-        <v>376.8</v>
+      <c r="C27" s="22">
+        <v>340.42</v>
       </c>
-      <c r="Y26" s="5">
-        <v>20</v>
-      </c>
-      <c r="Z26" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y26,$Y$3:$AA$13,COUNTIF($Y$17:Y26,Y26)+1,0)=0,NA(),VLOOKUP($Y26,$Y$3:$AA$13,COUNTIF($Y$17:Y26,Y26)+1,0)),NA())</f>
-        <v>30</v>
-      </c>
-      <c r="AA26" s="14"/>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B27" s="34">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B28" s="22">
         <v>0.2</v>
       </c>
-      <c r="C27" s="34">
-        <f>2713/10</f>
-        <v>271.3</v>
+      <c r="C28" s="22">
+        <v>244.93</v>
       </c>
-      <c r="Y27" s="5">
-        <v>25</v>
-      </c>
-      <c r="Z27" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y27,$Y$3:$AA$13,COUNTIF($Y$17:Y27,Y27)+1,0)=0,NA(),VLOOKUP($Y27,$Y$3:$AA$13,COUNTIF($Y$17:Y27,Y27)+1,0)),NA())</f>
-        <v>24.5</v>
-      </c>
-      <c r="AA27" s="14"/>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B28" s="34">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B29" s="22">
         <v>0.3</v>
       </c>
-      <c r="C28" s="34">
-        <f>1852/10</f>
-        <v>185.2</v>
+      <c r="C29" s="22">
+        <v>166.94</v>
       </c>
-      <c r="Y28" s="5">
-        <v>25</v>
-      </c>
-      <c r="Z28" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y28,$Y$3:$AA$13,COUNTIF($Y$17:Y28,Y28)+1,0)=0,NA(),VLOOKUP($Y28,$Y$3:$AA$13,COUNTIF($Y$17:Y28,Y28)+1,0)),NA())</f>
-        <v>35</v>
-      </c>
-      <c r="AA28" s="14"/>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B29" s="34">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B30" s="22">
         <v>0.4</v>
       </c>
-      <c r="C29" s="34">
-        <f>1182/10</f>
-        <v>118.2</v>
+      <c r="C30" s="22">
+        <v>106.45</v>
       </c>
-      <c r="Y29" s="5">
-        <v>30</v>
-      </c>
-      <c r="Z29" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y29,$Y$3:$AA$13,COUNTIF($Y$17:Y29,Y29)+1,0)=0,NA(),VLOOKUP($Y29,$Y$3:$AA$13,COUNTIF($Y$17:Y29,Y29)+1,0)),NA())</f>
-        <v>28</v>
-      </c>
-      <c r="AA29" s="14"/>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B30" s="34">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B31" s="22">
         <v>0.5</v>
       </c>
-      <c r="C30" s="34">
-        <f>706/10</f>
-        <v>70.599999999999994</v>
+      <c r="C31" s="22">
+        <v>63.46</v>
       </c>
-      <c r="Y30" s="5">
-        <v>30</v>
-      </c>
-      <c r="Z30" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y30,$Y$3:$AA$13,COUNTIF($Y$17:Y30,Y30)+1,0)=0,NA(),VLOOKUP($Y30,$Y$3:$AA$13,COUNTIF($Y$17:Y30,Y30)+1,0)),NA())</f>
-        <v>30</v>
-      </c>
-      <c r="AA30" s="14"/>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B31" s="34">
+    <row r="32" spans="2:25" x14ac:dyDescent="0.75">
+      <c r="B32" s="22">
         <v>0.6</v>
       </c>
-      <c r="C31" s="34">
-        <f>412/10</f>
-        <v>41.2</v>
+      <c r="C32" s="22">
+        <v>37.97</v>
       </c>
-      <c r="Y31" s="5">
-        <v>35</v>
-      </c>
-      <c r="Z31" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y31,$Y$3:$AA$13,COUNTIF($Y$17:Y31,Y31)+1,0)=0,NA(),VLOOKUP($Y31,$Y$3:$AA$13,COUNTIF($Y$17:Y31,Y31)+1,0)),NA())</f>
-        <v>31.5</v>
-      </c>
-      <c r="AA31" s="14"/>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B32" s="35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B33" s="23">
         <v>0.7</v>
       </c>
-      <c r="C32" s="35">
-        <f>330/10</f>
-        <v>33</v>
+      <c r="C33" s="23">
+        <v>29.98</v>
       </c>
-      <c r="Y32" s="5">
-        <v>35</v>
-      </c>
-      <c r="Z32" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y32,$Y$3:$AA$13,COUNTIF($Y$17:Y32,Y32)+1,0)=0,NA(),VLOOKUP($Y32,$Y$3:$AA$13,COUNTIF($Y$17:Y32,Y32)+1,0)),NA())</f>
-        <v>43</v>
-      </c>
-      <c r="AA32" s="14"/>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B33" s="34">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B34" s="22">
         <v>0.8</v>
       </c>
-      <c r="C33" s="34">
-        <f>430/10</f>
-        <v>43</v>
+      <c r="C34" s="22">
+        <f>39.49</f>
+        <v>39.49</v>
       </c>
-      <c r="Y33" s="5">
-        <v>40</v>
-      </c>
-      <c r="Z33" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y33,$Y$3:$AA$13,COUNTIF($Y$17:Y33,Y33)+1,0)=0,NA(),VLOOKUP($Y33,$Y$3:$AA$13,COUNTIF($Y$17:Y33,Y33)+1,0)),NA())</f>
-        <v>35</v>
-      </c>
-      <c r="AA33" s="14"/>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B34" s="34">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B35" s="22">
         <v>0.9</v>
       </c>
-      <c r="C34" s="34">
-        <f>724/10</f>
-        <v>72.400000000000006</v>
+      <c r="C35" s="22">
+        <v>66.5</v>
       </c>
-      <c r="Y34" s="5">
-        <v>40</v>
-      </c>
-      <c r="Z34" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y34,$Y$3:$AA$13,COUNTIF($Y$17:Y34,Y34)+1,0)=0,NA(),VLOOKUP($Y34,$Y$3:$AA$13,COUNTIF($Y$17:Y34,Y34)+1,0)),NA())</f>
-        <v>41</v>
-      </c>
-      <c r="AA34" s="14"/>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B35" s="34">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B36" s="22">
         <v>1</v>
       </c>
-      <c r="C35" s="34">
-        <f>1209/10</f>
-        <v>120.9</v>
+      <c r="C36" s="22">
+        <v>111.01</v>
       </c>
-      <c r="Y35" s="5">
-        <v>45</v>
-      </c>
-      <c r="Z35" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y35,$Y$3:$AA$13,COUNTIF($Y$17:Y35,Y35)+1,0)=0,NA(),VLOOKUP($Y35,$Y$3:$AA$13,COUNTIF($Y$17:Y35,Y35)+1,0)),NA())</f>
-        <v>38.5</v>
-      </c>
-      <c r="AA35" s="14"/>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B36" s="34">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B37" s="22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C36" s="34">
-        <f>1888/10</f>
-        <v>188.8</v>
+      <c r="C37" s="22">
+        <v>173.02</v>
       </c>
-      <c r="Y36" s="5">
-        <v>45</v>
-      </c>
-      <c r="Z36" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y36,$Y$3:$AA$13,COUNTIF($Y$17:Y36,Y36)+1,0)=0,NA(),VLOOKUP($Y36,$Y$3:$AA$13,COUNTIF($Y$17:Y36,Y36)+1,0)),NA())</f>
-        <v>44</v>
-      </c>
-      <c r="AA36" s="14"/>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B37" s="34">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B38" s="22">
         <v>1.2</v>
       </c>
-      <c r="C37" s="34">
-        <f>2758/10</f>
-        <v>275.8</v>
+      <c r="C38" s="22">
+        <v>252.52</v>
       </c>
-      <c r="Y37" s="5">
-        <v>50</v>
-      </c>
-      <c r="Z37" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y37,$Y$3:$AA$13,COUNTIF($Y$17:Y37,Y37)+1,0)=0,NA(),VLOOKUP($Y37,$Y$3:$AA$13,COUNTIF($Y$17:Y37,Y37)+1,0)),NA())</f>
-        <v>42</v>
-      </c>
-      <c r="AA37" s="14"/>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B38" s="34">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B39" s="22">
         <v>1.3</v>
       </c>
-      <c r="C38" s="34">
-        <f>3822/10</f>
-        <v>382.2</v>
+      <c r="C39" s="22">
+        <f>349.53</f>
+        <v>349.53</v>
       </c>
-      <c r="Y38" s="5">
-        <v>50</v>
-      </c>
-      <c r="Z38" s="5">
-        <f>IF($AB$6=TRUE,IF(VLOOKUP($Y38,$Y$3:$AA$13,COUNTIF($Y$17:Y38,Y38)+1,0)=0,NA(),VLOOKUP($Y38,$Y$3:$AA$13,COUNTIF($Y$17:Y38,Y38)+1,0)),NA())</f>
-        <v>34</v>
-      </c>
-      <c r="AA38" s="14"/>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B39" s="34">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B40" s="22">
         <v>1.4</v>
       </c>
-      <c r="C39" s="34">
-        <f>5077/10</f>
-        <v>507.7</v>
+      <c r="C40" s="22">
+        <v>464.04</v>
       </c>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B40" s="34">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B41" s="22">
         <v>1.5</v>
       </c>
-      <c r="C40" s="34">
-        <f>6526/10</f>
-        <v>652.6</v>
+      <c r="C41" s="22">
+        <v>496.05</v>
       </c>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.75">
-      <c r="B41" s="34">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.75">
+      <c r="B42" s="22">
         <v>1.6</v>
       </c>
-      <c r="C41" s="34">
-        <f>8166/10</f>
-        <v>816.6</v>
+      <c r="C42" s="22">
+        <v>745.56</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="Y1:AB1"/>
+  <mergeCells count="7">
+    <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:L3"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="O3:P3"/>
+    <mergeCell ref="X1:Y1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -31578,7 +32617,7 @@
                   </from>
                   <to>
                     <xdr:col>9</xdr:col>
-                    <xdr:colOff>304800</xdr:colOff>
+                    <xdr:colOff>314325</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -31591,4 +32630,217 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79033A87-5D12-45E5-B76B-F23C71BDA033}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>-10</v>
+      </c>
+      <c r="B2">
+        <f xml:space="preserve"> A2 *A2</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>-9</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B22" si="0" xml:space="preserve"> A3 *A3</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>-8</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>-7</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>-6</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>-5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>-4</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>-3</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>-2</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>-1</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>